<commit_message>
Alot fixing quoatation fully implemented
</commit_message>
<xml_diff>
--- a/AppData/Templates/Excel.xlsx
+++ b/AppData/Templates/Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ECO ENTERPRISES\eco enterprises\AppData\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC25D7C-DD87-478C-9B3C-3C73151491D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D331281A-2A24-4CBB-B2B1-C7B4802315A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,6 +600,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,8 +629,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="6" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -620,30 +639,11 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="6" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1020,32 +1020,32 @@
   <sheetData>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
+      <c r="A5" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
@@ -1053,57 +1053,57 @@
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="44" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
@@ -1266,12 +1266,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="17">
         <f t="shared" ref="E15:J15" si="0">SUM(E10:E14)</f>
         <v>0</v>
@@ -1298,32 +1298,25 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="41"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="41"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="56"/>
+      <c r="B21" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="F7:J7"/>
@@ -1334,6 +1327,13 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1344,7 +1344,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,8 +1466,8 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="33"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1609,6 +1609,7 @@
         <v>780</v>
       </c>
       <c r="H20" s="8">
+        <f>G20*E20</f>
         <v>780</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Thak gya hu vro
</commit_message>
<xml_diff>
--- a/AppData/Templates/Excel.xlsx
+++ b/AppData/Templates/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ECO ENTERPRISES\eco enterprises\AppData\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D331281A-2A24-4CBB-B2B1-C7B4802315A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA541454-1B7C-474F-93FD-E820839F6612}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>Subject:      Bill for subject_line:</t>
-  </si>
-  <si>
     <t>Services</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>Subject:      Bill for Repairing of Split Air Conditioners:</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -601,26 +601,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,6 +609,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="6" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,11 +621,30 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="43" fontId="6" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1020,32 +1021,32 @@
   <sheetData>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="53"/>
+      <c r="A5" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="48"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
@@ -1053,57 +1054,57 @@
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="48"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="46"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="G8" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="58" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
@@ -1266,12 +1267,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="17">
         <f t="shared" ref="E15:J15" si="0">SUM(E10:E14)</f>
         <v>0</v>
@@ -1298,25 +1299,32 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="57"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="57"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="41"/>
+      <c r="B21" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="F7:J7"/>
@@ -1327,13 +1335,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1344,7 +1345,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,11 +1365,11 @@
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="4"/>
       <c r="H2" s="2"/>
     </row>
@@ -1378,11 +1379,11 @@
       <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
       <c r="G3" s="4"/>
       <c r="H3" s="2"/>
     </row>
@@ -1392,11 +1393,11 @@
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="4"/>
       <c r="H4" s="2"/>
     </row>
@@ -1406,11 +1407,11 @@
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
       <c r="G5" s="4"/>
       <c r="H5" s="2"/>
     </row>
@@ -1465,9 +1466,9 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="33"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1485,16 +1486,16 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
+      <c r="A12" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
@@ -1507,37 +1508,37 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
+      <c r="A14" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="64"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="38" t="s">
+      <c r="F15" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="G15" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="H15" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1568,7 +1569,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="31">
         <f>SUM(H16:H17)</f>
@@ -1583,7 +1584,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="31">
         <f>H18*0.16</f>
@@ -1595,7 +1596,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="28"/>
@@ -1603,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" s="7">
         <v>780</v>
@@ -1626,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" s="7">
         <v>0</v>
@@ -1718,7 +1719,7 @@
     </row>
     <row r="43" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>